<commit_message>
The bacteria name is incorrect in record number 411 in supplementary_table_3, so I fixed that into Bacillus_cereus_ATCC_14579
</commit_message>
<xml_diff>
--- a/manuscript/supplementary-material/Supplementary Table 3.xlsx
+++ b/manuscript/supplementary-material/Supplementary Table 3.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="539">
   <si>
     <t>Species</t>
   </si>
@@ -1547,13 +1547,16 @@
     <t>CP001503.2</t>
   </si>
   <si>
+    <t>Bacillus_cereus_ATCC_14579</t>
+  </si>
+  <si>
+    <t>AE016877.1</t>
+  </si>
+  <si>
+    <t>ERR031734</t>
+  </si>
+  <si>
     <t>Bacillus_cereus_ATCC_10987</t>
-  </si>
-  <si>
-    <t>AE016877.1</t>
-  </si>
-  <si>
-    <t>ERR031734</t>
   </si>
   <si>
     <t>AE017194.1</t>
@@ -1642,6 +1645,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -1725,27 +1729,27 @@
   </sheetPr>
   <dimension ref="A1:L429"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A387" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A411" activeCellId="0" pane="topLeft" sqref="A411"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6941176470588"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4862745098039"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.521568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5137254901961"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.4470588235294"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8862745098039"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.356862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.6666666666667"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.25098039215686"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.9843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5411764705882"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5960784313726"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5137254901961"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0745098039216"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.9529411764706"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.4470588235294"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.7843137254902"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.29803921568628"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.0901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1783,7 +1787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
@@ -1821,7 +1825,7 @@
         <v>0.954668374375961</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
@@ -1859,7 +1863,7 @@
         <v>0.941014333338516</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
@@ -1897,7 +1901,7 @@
         <v>0.981264936969954</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
@@ -1935,7 +1939,7 @@
         <v>0.958573175614203</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
@@ -1973,7 +1977,7 @@
         <v>0.952505579584536</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
@@ -2011,7 +2015,7 @@
         <v>0.957477564880534</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>21</v>
       </c>
@@ -2049,7 +2053,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>21</v>
       </c>
@@ -2087,7 +2091,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>21</v>
       </c>
@@ -2125,7 +2129,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>21</v>
       </c>
@@ -2163,7 +2167,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>30</v>
       </c>
@@ -2201,7 +2205,7 @@
         <v>0.430664564781892</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>30</v>
       </c>
@@ -2239,7 +2243,7 @@
         <v>0.0557619956536407</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>30</v>
       </c>
@@ -2277,7 +2281,7 @@
         <v>0.0550752720373589</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>30</v>
       </c>
@@ -2315,7 +2319,7 @@
         <v>0.940791493950757</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>30</v>
       </c>
@@ -2353,7 +2357,7 @@
         <v>0.915058363773324</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>30</v>
       </c>
@@ -2369,9 +2373,6 @@
       <c r="E17" s="0" t="n">
         <v>0.6506846</v>
       </c>
-      <c r="F17" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="G17" s="0" t="n">
         <v>1</v>
       </c>
@@ -2391,7 +2392,7 @@
         <v>0.946446512506185</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>30</v>
       </c>
@@ -2429,7 +2430,7 @@
         <v>0.91967449008299</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>30</v>
       </c>
@@ -2467,7 +2468,7 @@
         <v>0.80116940605101</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>30</v>
       </c>
@@ -2505,7 +2506,7 @@
         <v>0.907537296562147</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>46</v>
       </c>
@@ -2543,7 +2544,7 @@
         <v>0.104361944126106</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>46</v>
       </c>
@@ -2581,7 +2582,7 @@
         <v>0.0741965777387339</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>46</v>
       </c>
@@ -2619,7 +2620,7 @@
         <v>0.0525566272515136</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>46</v>
       </c>
@@ -2657,7 +2658,7 @@
         <v>0.0544551686357303</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
         <v>46</v>
       </c>
@@ -2695,7 +2696,7 @@
         <v>0.0764527617854425</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
         <v>46</v>
       </c>
@@ -2733,7 +2734,7 @@
         <v>0.0338529064246929</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
         <v>46</v>
       </c>
@@ -2771,7 +2772,7 @@
         <v>0.0326918633863267</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>46</v>
       </c>
@@ -2809,7 +2810,7 @@
         <v>0.0387529682747282</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
         <v>57</v>
       </c>
@@ -2847,7 +2848,7 @@
         <v>0.585481976636494</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
         <v>57</v>
       </c>
@@ -2885,7 +2886,7 @@
         <v>0.631591598041012</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
         <v>57</v>
       </c>
@@ -2923,7 +2924,7 @@
         <v>0.612680358474676</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
         <v>57</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>0.628207116173596</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
         <v>57</v>
       </c>
@@ -2999,7 +3000,7 @@
         <v>0.757513170668959</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
         <v>57</v>
       </c>
@@ -3037,7 +3038,7 @@
         <v>0.72457260317764</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
         <v>57</v>
       </c>
@@ -3075,7 +3076,7 @@
         <v>0.791092411615243</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
         <v>57</v>
       </c>
@@ -3113,7 +3114,7 @@
         <v>0.688785028431101</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
         <v>68</v>
       </c>
@@ -3151,7 +3152,7 @@
         <v>0.311388904452787</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
         <v>68</v>
       </c>
@@ -3189,7 +3190,7 @@
         <v>0.0695269710532746</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
         <v>68</v>
       </c>
@@ -3227,7 +3228,7 @@
         <v>0.3483094423842</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
         <v>68</v>
       </c>
@@ -3265,7 +3266,7 @@
         <v>0.199575640743664</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
         <v>75</v>
       </c>
@@ -3303,7 +3304,7 @@
         <v>0.164284429616839</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
         <v>75</v>
       </c>
@@ -3341,7 +3342,7 @@
         <v>0.021748499646889</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
         <v>75</v>
       </c>
@@ -3379,7 +3380,7 @@
         <v>0.102545685199207</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
         <v>75</v>
       </c>
@@ -3417,7 +3418,7 @@
         <v>0.1223322776715</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
         <v>75</v>
       </c>
@@ -3455,7 +3456,7 @@
         <v>0.955643642286924</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
         <v>75</v>
       </c>
@@ -3493,7 +3494,7 @@
         <v>0.942787636013627</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
         <v>75</v>
       </c>
@@ -3531,7 +3532,7 @@
         <v>0.966694258791445</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
         <v>86</v>
       </c>
@@ -3569,7 +3570,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
         <v>86</v>
       </c>
@@ -3607,7 +3608,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
         <v>86</v>
       </c>
@@ -3645,7 +3646,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
         <v>86</v>
       </c>
@@ -3683,7 +3684,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="0" t="s">
         <v>86</v>
       </c>
@@ -3721,7 +3722,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
         <v>86</v>
       </c>
@@ -3759,7 +3760,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
         <v>94</v>
       </c>
@@ -3797,7 +3798,7 @@
         <v>0.950077346575427</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
         <v>94</v>
       </c>
@@ -3835,7 +3836,7 @@
         <v>0.948843030284497</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
         <v>94</v>
       </c>
@@ -3873,7 +3874,7 @@
         <v>0.907611691910058</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="A57" s="0" t="s">
         <v>94</v>
       </c>
@@ -3911,7 +3912,7 @@
         <v>0.940999971514855</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="58">
       <c r="A58" s="0" t="s">
         <v>94</v>
       </c>
@@ -3949,7 +3950,7 @@
         <v>0.950077346575427</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
         <v>94</v>
       </c>
@@ -3987,7 +3988,7 @@
         <v>0.948843030284497</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
         <v>94</v>
       </c>
@@ -4025,7 +4026,7 @@
         <v>0.907611691910058</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
         <v>94</v>
       </c>
@@ -4063,7 +4064,7 @@
         <v>0.940999971514855</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="62">
       <c r="A62" s="0" t="s">
         <v>102</v>
       </c>
@@ -4101,7 +4102,7 @@
         <v>0.304912875609049</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="63">
       <c r="A63" s="0" t="s">
         <v>102</v>
       </c>
@@ -4139,7 +4140,7 @@
         <v>0.010864727795353</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="64">
       <c r="A64" s="0" t="s">
         <v>102</v>
       </c>
@@ -4177,7 +4178,7 @@
         <v>0.175087903246778</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="A65" s="0" t="s">
         <v>110</v>
       </c>
@@ -4215,7 +4216,7 @@
         <v>0.409005249026046</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="66">
       <c r="A66" s="0" t="s">
         <v>110</v>
       </c>
@@ -4253,7 +4254,7 @@
         <v>0.436297236002059</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="67">
       <c r="A67" s="0" t="s">
         <v>115</v>
       </c>
@@ -4291,7 +4292,7 @@
         <v>0.537058323754311</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
         <v>115</v>
       </c>
@@ -4329,7 +4330,7 @@
         <v>0.361788148319279</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="69">
       <c r="A69" s="0" t="s">
         <v>115</v>
       </c>
@@ -4367,7 +4368,7 @@
         <v>0.926810508060322</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="A70" s="0" t="s">
         <v>115</v>
       </c>
@@ -4405,7 +4406,7 @@
         <v>0.9924779639431</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="71">
       <c r="A71" s="0" t="s">
         <v>115</v>
       </c>
@@ -4443,7 +4444,7 @@
         <v>0.991780553382021</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="A72" s="0" t="s">
         <v>115</v>
       </c>
@@ -4481,7 +4482,7 @@
         <v>0.846968205363719</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="73">
       <c r="A73" s="0" t="s">
         <v>115</v>
       </c>
@@ -4519,7 +4520,7 @@
         <v>0.764454914837258</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="74">
       <c r="A74" s="0" t="s">
         <v>115</v>
       </c>
@@ -4557,7 +4558,7 @@
         <v>0.991314928177675</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="75">
       <c r="A75" s="0" t="s">
         <v>128</v>
       </c>
@@ -4595,7 +4596,7 @@
         <v>0.924412156333826</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
         <v>128</v>
       </c>
@@ -4633,7 +4634,7 @@
         <v>0.942330079730382</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="77">
       <c r="A77" s="0" t="s">
         <v>128</v>
       </c>
@@ -4671,7 +4672,7 @@
         <v>0.939069453997557</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="78">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="78">
       <c r="A78" s="0" t="s">
         <v>128</v>
       </c>
@@ -4709,7 +4710,7 @@
         <v>0.946344965542747</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="79">
       <c r="A79" s="0" t="s">
         <v>128</v>
       </c>
@@ -4747,7 +4748,7 @@
         <v>0.932792779381132</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="80">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
         <v>128</v>
       </c>
@@ -4785,7 +4786,7 @@
         <v>0.93200992198921</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="81">
       <c r="A81" s="0" t="s">
         <v>128</v>
       </c>
@@ -4823,7 +4824,7 @@
         <v>0.92080123261779</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="82">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="82">
       <c r="A82" s="0" t="s">
         <v>128</v>
       </c>
@@ -4861,7 +4862,7 @@
         <v>0.944848417560584</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="83">
       <c r="A83" s="0" t="s">
         <v>128</v>
       </c>
@@ -4899,7 +4900,7 @@
         <v>0.477630147373974</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="84">
       <c r="A84" s="0" t="s">
         <v>128</v>
       </c>
@@ -4937,7 +4938,7 @@
         <v>0.492325321914297</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="85">
       <c r="A85" s="0" t="s">
         <v>141</v>
       </c>
@@ -4975,7 +4976,7 @@
         <v>0.643527120091304</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="86">
       <c r="A86" s="0" t="s">
         <v>141</v>
       </c>
@@ -5013,7 +5014,7 @@
         <v>0.643491312960885</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="87">
       <c r="A87" s="0" t="s">
         <v>141</v>
       </c>
@@ -5051,7 +5052,7 @@
         <v>0.659065012859329</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="88">
       <c r="A88" s="0" t="s">
         <v>141</v>
       </c>
@@ -5089,7 +5090,7 @@
         <v>0.65991808576166</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="89">
       <c r="A89" s="0" t="s">
         <v>148</v>
       </c>
@@ -5127,7 +5128,7 @@
         <v>0.98434909286137</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="90">
       <c r="A90" s="0" t="s">
         <v>148</v>
       </c>
@@ -5165,7 +5166,7 @@
         <v>0.986440321926752</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="91">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="91">
       <c r="A91" s="0" t="s">
         <v>153</v>
       </c>
@@ -5203,7 +5204,7 @@
         <v>0.215606771590327</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="92">
       <c r="A92" s="0" t="s">
         <v>153</v>
       </c>
@@ -5241,7 +5242,7 @@
         <v>0.298103384537538</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="93">
       <c r="A93" s="0" t="s">
         <v>153</v>
       </c>
@@ -5279,7 +5280,7 @@
         <v>0.95071011904533</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="94">
       <c r="A94" s="0" t="s">
         <v>159</v>
       </c>
@@ -5317,7 +5318,7 @@
         <v>0.0561651217739802</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="95">
       <c r="A95" s="0" t="s">
         <v>159</v>
       </c>
@@ -5355,7 +5356,7 @@
         <v>0.131498837945538</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="96">
       <c r="A96" s="0" t="s">
         <v>159</v>
       </c>
@@ -5393,7 +5394,7 @@
         <v>0.0429569868090408</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="97">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="97">
       <c r="A97" s="0" t="s">
         <v>159</v>
       </c>
@@ -5431,7 +5432,7 @@
         <v>0.093390200649892</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="98">
       <c r="A98" s="0" t="s">
         <v>159</v>
       </c>
@@ -5469,7 +5470,7 @@
         <v>0.240218784641582</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="99">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="99">
       <c r="A99" s="0" t="s">
         <v>159</v>
       </c>
@@ -5507,7 +5508,7 @@
         <v>0.0770594213281746</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="100">
       <c r="A100" s="0" t="s">
         <v>159</v>
       </c>
@@ -5545,7 +5546,7 @@
         <v>0.0327764465250503</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="101">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="101">
       <c r="A101" s="0" t="s">
         <v>159</v>
       </c>
@@ -5583,7 +5584,7 @@
         <v>0.0634423602338883</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="102">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="102">
       <c r="A102" s="0" t="s">
         <v>159</v>
       </c>
@@ -5621,7 +5622,7 @@
         <v>0.0793008226624285</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="103">
       <c r="A103" s="0" t="s">
         <v>159</v>
       </c>
@@ -5659,7 +5660,7 @@
         <v>0.0537069940495316</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="104">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="104">
       <c r="A104" s="0" t="s">
         <v>172</v>
       </c>
@@ -5697,7 +5698,7 @@
         <v>0.246858178859992</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="105">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="105">
       <c r="A105" s="0" t="s">
         <v>172</v>
       </c>
@@ -5735,7 +5736,7 @@
         <v>0.247045244090488</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="106">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="106">
       <c r="A106" s="0" t="s">
         <v>172</v>
       </c>
@@ -5773,7 +5774,7 @@
         <v>0.247028555814251</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="107">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="107">
       <c r="A107" s="0" t="s">
         <v>172</v>
       </c>
@@ -5811,7 +5812,7 @@
         <v>0.243891426809997</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="108">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="108">
       <c r="A108" s="0" t="s">
         <v>172</v>
       </c>
@@ -5849,7 +5850,7 @@
         <v>0.249072954196598</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="109">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="109">
       <c r="A109" s="0" t="s">
         <v>180</v>
       </c>
@@ -5887,7 +5888,7 @@
         <v>0.969891714491924</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="110">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="110">
       <c r="A110" s="0" t="s">
         <v>180</v>
       </c>
@@ -5925,7 +5926,7 @@
         <v>0.945648131003725</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="111">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="111">
       <c r="A111" s="0" t="s">
         <v>180</v>
       </c>
@@ -5963,7 +5964,7 @@
         <v>0.94917939491754</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="112">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="112">
       <c r="A112" s="0" t="s">
         <v>180</v>
       </c>
@@ -6001,7 +6002,7 @@
         <v>0.98494255983796</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="113">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="113">
       <c r="A113" s="0" t="s">
         <v>180</v>
       </c>
@@ -6039,7 +6040,7 @@
         <v>0.983779325359626</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="114">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="114">
       <c r="A114" s="0" t="s">
         <v>180</v>
       </c>
@@ -6077,7 +6078,7 @@
         <v>0.968853208954664</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="115">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="115">
       <c r="A115" s="0" t="s">
         <v>180</v>
       </c>
@@ -6115,7 +6116,7 @@
         <v>7.67009844571355E-006</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="116">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="116">
       <c r="A116" s="0" t="s">
         <v>180</v>
       </c>
@@ -6153,7 +6154,7 @@
         <v>1.99283520939255E-005</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="117">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="117">
       <c r="A117" s="0" t="s">
         <v>180</v>
       </c>
@@ -6191,7 +6192,7 @@
         <v>0.00019936661736302</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="118">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="118">
       <c r="A118" s="0" t="s">
         <v>192</v>
       </c>
@@ -6229,7 +6230,7 @@
         <v>0.939152402160143</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="119">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="119">
       <c r="A119" s="0" t="s">
         <v>192</v>
       </c>
@@ -6267,7 +6268,7 @@
         <v>0.891202141165155</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="120">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="120">
       <c r="A120" s="0" t="s">
         <v>192</v>
       </c>
@@ -6305,7 +6306,7 @@
         <v>0.902405771266853</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="121">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="121">
       <c r="A121" s="0" t="s">
         <v>198</v>
       </c>
@@ -6343,7 +6344,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="122">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="122">
       <c r="A122" s="0" t="s">
         <v>201</v>
       </c>
@@ -6381,7 +6382,7 @@
         <v>0.947361901867051</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="123">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="123">
       <c r="A123" s="0" t="s">
         <v>201</v>
       </c>
@@ -6419,7 +6420,7 @@
         <v>0.949728587656751</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="124">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="124">
       <c r="A124" s="0" t="s">
         <v>201</v>
       </c>
@@ -6457,7 +6458,7 @@
         <v>0.947706705059646</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="125">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="125">
       <c r="A125" s="0" t="s">
         <v>201</v>
       </c>
@@ -6495,7 +6496,7 @@
         <v>0.964461748476068</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="126">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="126">
       <c r="A126" s="0" t="s">
         <v>201</v>
       </c>
@@ -6533,7 +6534,7 @@
         <v>0.824963791941498</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="127">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="127">
       <c r="A127" s="0" t="s">
         <v>201</v>
       </c>
@@ -6571,7 +6572,7 @@
         <v>0.824710351458915</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="128">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="128">
       <c r="A128" s="0" t="s">
         <v>201</v>
       </c>
@@ -6609,7 +6610,7 @@
         <v>0.973063582137207</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="129">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="129">
       <c r="A129" s="0" t="s">
         <v>201</v>
       </c>
@@ -6647,7 +6648,7 @@
         <v>0.995840665229164</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="130">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="130">
       <c r="A130" s="0" t="s">
         <v>201</v>
       </c>
@@ -6685,7 +6686,7 @@
         <v>0.971642840340016</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="131">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="131">
       <c r="A131" s="0" t="s">
         <v>201</v>
       </c>
@@ -6723,7 +6724,7 @@
         <v>0.920338457721637</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="132">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="132">
       <c r="A132" s="0" t="s">
         <v>201</v>
       </c>
@@ -6761,7 +6762,7 @@
         <v>0.877411759677229</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="133">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="133">
       <c r="A133" s="0" t="s">
         <v>201</v>
       </c>
@@ -6799,7 +6800,7 @@
         <v>0.939903760856512</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="134">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="134">
       <c r="A134" s="0" t="s">
         <v>201</v>
       </c>
@@ -6837,7 +6838,7 @@
         <v>0.934786541685135</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="135">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="135">
       <c r="A135" s="0" t="s">
         <v>201</v>
       </c>
@@ -6875,7 +6876,7 @@
         <v>0.951885753607726</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="136">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="136">
       <c r="A136" s="0" t="s">
         <v>201</v>
       </c>
@@ -6913,7 +6914,7 @@
         <v>0.957123523622047</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="137">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="137">
       <c r="A137" s="0" t="s">
         <v>201</v>
       </c>
@@ -6951,7 +6952,7 @@
         <v>0.93706470541639</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="138">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="138">
       <c r="A138" s="0" t="s">
         <v>201</v>
       </c>
@@ -6989,7 +6990,7 @@
         <v>0.896465394895305</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="139">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="139">
       <c r="A139" s="0" t="s">
         <v>201</v>
       </c>
@@ -7027,7 +7028,7 @@
         <v>0.951596455349942</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="140">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="140">
       <c r="A140" s="0" t="s">
         <v>201</v>
       </c>
@@ -7065,7 +7066,7 @@
         <v>0.925158920325682</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="141">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="141">
       <c r="A141" s="0" t="s">
         <v>201</v>
       </c>
@@ -7103,7 +7104,7 @@
         <v>0.935671312642494</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="142">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="142">
       <c r="A142" s="0" t="s">
         <v>201</v>
       </c>
@@ -7141,7 +7142,7 @@
         <v>0.98816743941745</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="143">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="143">
       <c r="A143" s="0" t="s">
         <v>201</v>
       </c>
@@ -7179,7 +7180,7 @@
         <v>0.948865682922108</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="144">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="144">
       <c r="A144" s="0" t="s">
         <v>201</v>
       </c>
@@ -7217,7 +7218,7 @@
         <v>0.975956368524013</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="145">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="145">
       <c r="A145" s="0" t="s">
         <v>201</v>
       </c>
@@ -7255,7 +7256,7 @@
         <v>0.956435269154546</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="146">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="146">
       <c r="A146" s="0" t="s">
         <v>201</v>
       </c>
@@ -7293,7 +7294,7 @@
         <v>0.946346371360181</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="147">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="147">
       <c r="A147" s="0" t="s">
         <v>201</v>
       </c>
@@ -7331,7 +7332,7 @@
         <v>0.902952282263541</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="148">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="148">
       <c r="A148" s="0" t="s">
         <v>201</v>
       </c>
@@ -7369,7 +7370,7 @@
         <v>0.95564781856817</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="149">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="149">
       <c r="A149" s="0" t="s">
         <v>201</v>
       </c>
@@ -7407,7 +7408,7 @@
         <v>0.96886959928393</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="150">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="150">
       <c r="A150" s="0" t="s">
         <v>201</v>
       </c>
@@ -7445,7 +7446,7 @@
         <v>0.92738994075967</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="151">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="151">
       <c r="A151" s="0" t="s">
         <v>201</v>
       </c>
@@ -7483,7 +7484,7 @@
         <v>0.936797627888386</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="152">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="152">
       <c r="A152" s="0" t="s">
         <v>201</v>
       </c>
@@ -7521,7 +7522,7 @@
         <v>0.935213475591013</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="153">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="153">
       <c r="A153" s="0" t="s">
         <v>201</v>
       </c>
@@ -7559,7 +7560,7 @@
         <v>0.971639772062327</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="154">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="154">
       <c r="A154" s="0" t="s">
         <v>201</v>
       </c>
@@ -7597,7 +7598,7 @@
         <v>0.924387769496034</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="155">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="155">
       <c r="A155" s="0" t="s">
         <v>201</v>
       </c>
@@ -7635,7 +7636,7 @@
         <v>0.968459723800551</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="156">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="156">
       <c r="A156" s="0" t="s">
         <v>201</v>
       </c>
@@ -7673,7 +7674,7 @@
         <v>0.954348823988079</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="157">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="157">
       <c r="A157" s="0" t="s">
         <v>201</v>
       </c>
@@ -7711,7 +7712,7 @@
         <v>0.928279352226721</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="158">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="158">
       <c r="A158" s="0" t="s">
         <v>201</v>
       </c>
@@ -7749,7 +7750,7 @@
         <v>0.987174177940248</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="159">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="159">
       <c r="A159" s="0" t="s">
         <v>201</v>
       </c>
@@ -7787,7 +7788,7 @@
         <v>0.952134410274082</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="160">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="160">
       <c r="A160" s="0" t="s">
         <v>201</v>
       </c>
@@ -7825,7 +7826,7 @@
         <v>0.967919542645988</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="161">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="161">
       <c r="A161" s="0" t="s">
         <v>201</v>
       </c>
@@ -7863,7 +7864,7 @@
         <v>0.94905892234006</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="162">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="162">
       <c r="A162" s="0" t="s">
         <v>201</v>
       </c>
@@ -7901,7 +7902,7 @@
         <v>0.943133901291425</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="163">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="163">
       <c r="A163" s="0" t="s">
         <v>201</v>
       </c>
@@ -7939,7 +7940,7 @@
         <v>0.901298995056064</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="164">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="164">
       <c r="A164" s="0" t="s">
         <v>201</v>
       </c>
@@ -7977,7 +7978,7 @@
         <v>0.940124506843339</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="165">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="165">
       <c r="A165" s="0" t="s">
         <v>201</v>
       </c>
@@ -8015,7 +8016,7 @@
         <v>0.874214059918736</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="166">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="166">
       <c r="A166" s="0" t="s">
         <v>201</v>
       </c>
@@ -8053,7 +8054,7 @@
         <v>0.990901576852782</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="167">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="167">
       <c r="A167" s="0" t="s">
         <v>201</v>
       </c>
@@ -8091,7 +8092,7 @@
         <v>0.973567318481465</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="168">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="168">
       <c r="A168" s="0" t="s">
         <v>201</v>
       </c>
@@ -8129,7 +8130,7 @@
         <v>0.928869503413408</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="169">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="169">
       <c r="A169" s="0" t="s">
         <v>201</v>
       </c>
@@ -8167,7 +8168,7 @@
         <v>0.949093764583717</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="170">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="170">
       <c r="A170" s="0" t="s">
         <v>201</v>
       </c>
@@ -8205,7 +8206,7 @@
         <v>0.971785525493189</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="171">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="171">
       <c r="A171" s="0" t="s">
         <v>201</v>
       </c>
@@ -8243,7 +8244,7 @@
         <v>0.938389342973559</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="172">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="172">
       <c r="A172" s="0" t="s">
         <v>201</v>
       </c>
@@ -8281,7 +8282,7 @@
         <v>0.948631985837968</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="173">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="173">
       <c r="A173" s="0" t="s">
         <v>201</v>
       </c>
@@ -8319,7 +8320,7 @@
         <v>0.948492689352551</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="174">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="174">
       <c r="A174" s="0" t="s">
         <v>201</v>
       </c>
@@ -8357,7 +8358,7 @@
         <v>0.941677969385778</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="175">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="175">
       <c r="A175" s="0" t="s">
         <v>201</v>
       </c>
@@ -8395,7 +8396,7 @@
         <v>0.925857260393951</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="176">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="176">
       <c r="A176" s="0" t="s">
         <v>201</v>
       </c>
@@ -8433,7 +8434,7 @@
         <v>0.87589059687432</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="177">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="177">
       <c r="A177" s="0" t="s">
         <v>201</v>
       </c>
@@ -8471,7 +8472,7 @@
         <v>0.955008630976174</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="178">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="178">
       <c r="A178" s="0" t="s">
         <v>201</v>
       </c>
@@ -8509,7 +8510,7 @@
         <v>0.895924452490537</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="179">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="179">
       <c r="A179" s="0" t="s">
         <v>201</v>
       </c>
@@ -8547,7 +8548,7 @@
         <v>0.964123843419592</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="180">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="180">
       <c r="A180" s="0" t="s">
         <v>201</v>
       </c>
@@ -8585,7 +8586,7 @@
         <v>0.919867476734363</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="181">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="181">
       <c r="A181" s="0" t="s">
         <v>201</v>
       </c>
@@ -8623,7 +8624,7 @@
         <v>0.976681980789661</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="182">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="182">
       <c r="A182" s="0" t="s">
         <v>201</v>
       </c>
@@ -8661,7 +8662,7 @@
         <v>0.958060653451748</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="183">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="183">
       <c r="A183" s="0" t="s">
         <v>201</v>
       </c>
@@ -8699,7 +8700,7 @@
         <v>0.957911173024312</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="184">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="184">
       <c r="A184" s="0" t="s">
         <v>201</v>
       </c>
@@ -8737,7 +8738,7 @@
         <v>0.949874079658078</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="185">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="185">
       <c r="A185" s="0" t="s">
         <v>201</v>
       </c>
@@ -8775,7 +8776,7 @@
         <v>0.966180517737045</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="186">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="186">
       <c r="A186" s="0" t="s">
         <v>201</v>
       </c>
@@ -8813,7 +8814,7 @@
         <v>0.972663790008344</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="187">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="187">
       <c r="A187" s="0" t="s">
         <v>201</v>
       </c>
@@ -8851,7 +8852,7 @@
         <v>0.926443652851478</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="188">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="188">
       <c r="A188" s="0" t="s">
         <v>201</v>
       </c>
@@ -8889,7 +8890,7 @@
         <v>0.881848440919437</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="189">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="189">
       <c r="A189" s="0" t="s">
         <v>201</v>
       </c>
@@ -8927,7 +8928,7 @@
         <v>0.965356927795778</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="190">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="190">
       <c r="A190" s="0" t="s">
         <v>201</v>
       </c>
@@ -8965,7 +8966,7 @@
         <v>0.948558026119583</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="191">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="191">
       <c r="A191" s="0" t="s">
         <v>201</v>
       </c>
@@ -9003,7 +9004,7 @@
         <v>0.976336867438898</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="192">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="192">
       <c r="A192" s="0" t="s">
         <v>201</v>
       </c>
@@ -9041,7 +9042,7 @@
         <v>0.987929172163698</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="193">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="193">
       <c r="A193" s="0" t="s">
         <v>201</v>
       </c>
@@ -9079,7 +9080,7 @@
         <v>0.976981409058906</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="194">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="194">
       <c r="A194" s="0" t="s">
         <v>201</v>
       </c>
@@ -9117,7 +9118,7 @@
         <v>0.968725390260032</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="195">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="195">
       <c r="A195" s="0" t="s">
         <v>201</v>
       </c>
@@ -9155,7 +9156,7 @@
         <v>0.923898509423958</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="196">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="196">
       <c r="A196" s="0" t="s">
         <v>201</v>
       </c>
@@ -9193,7 +9194,7 @@
         <v>0.948699920830309</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="197">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="197">
       <c r="A197" s="0" t="s">
         <v>201</v>
       </c>
@@ -9231,7 +9232,7 @@
         <v>0.992704512588776</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="198">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="198">
       <c r="A198" s="0" t="s">
         <v>201</v>
       </c>
@@ -9269,7 +9270,7 @@
         <v>0.947361901867051</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="199">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="199">
       <c r="A199" s="0" t="s">
         <v>201</v>
       </c>
@@ -9307,7 +9308,7 @@
         <v>0.973063582137207</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="200">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="200">
       <c r="A200" s="0" t="s">
         <v>201</v>
       </c>
@@ -9345,7 +9346,7 @@
         <v>0.995840665229164</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="201">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="201">
       <c r="A201" s="0" t="s">
         <v>201</v>
       </c>
@@ -9383,7 +9384,7 @@
         <v>0.877411759677229</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="202">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="202">
       <c r="A202" s="0" t="s">
         <v>201</v>
       </c>
@@ -9421,7 +9422,7 @@
         <v>0.957123523622047</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="203">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="203">
       <c r="A203" s="0" t="s">
         <v>201</v>
       </c>
@@ -9459,7 +9460,7 @@
         <v>0.98816743941745</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="204">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="204">
       <c r="A204" s="0" t="s">
         <v>201</v>
       </c>
@@ -9497,7 +9498,7 @@
         <v>0.975956368524013</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="205">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="205">
       <c r="A205" s="0" t="s">
         <v>201</v>
       </c>
@@ -9535,7 +9536,7 @@
         <v>0.987174177940248</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="206">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="206">
       <c r="A206" s="0" t="s">
         <v>201</v>
       </c>
@@ -9573,7 +9574,7 @@
         <v>0.990901576852782</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="207">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="207">
       <c r="A207" s="0" t="s">
         <v>201</v>
       </c>
@@ -9611,7 +9612,7 @@
         <v>0.973567318481465</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="208">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="208">
       <c r="A208" s="0" t="s">
         <v>201</v>
       </c>
@@ -9649,7 +9650,7 @@
         <v>0.948492689352551</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="209">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="209">
       <c r="A209" s="0" t="s">
         <v>201</v>
       </c>
@@ -9687,7 +9688,7 @@
         <v>0.957911173024312</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="210">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="210">
       <c r="A210" s="0" t="s">
         <v>201</v>
       </c>
@@ -9725,7 +9726,7 @@
         <v>0.881848440919437</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="211">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="211">
       <c r="A211" s="0" t="s">
         <v>201</v>
       </c>
@@ -9763,7 +9764,7 @@
         <v>0.976336867438898</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="212">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="212">
       <c r="A212" s="0" t="s">
         <v>201</v>
       </c>
@@ -9801,7 +9802,7 @@
         <v>0.987929172163698</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="213">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="213">
       <c r="A213" s="0" t="s">
         <v>201</v>
       </c>
@@ -9839,7 +9840,7 @@
         <v>0.992704512588776</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="214">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="214">
       <c r="A214" s="0" t="s">
         <v>281</v>
       </c>
@@ -9877,7 +9878,7 @@
         <v>0.164164010599212</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="215">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="215">
       <c r="A215" s="0" t="s">
         <v>281</v>
       </c>
@@ -9915,7 +9916,7 @@
         <v>0.051703991984386</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="216">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="216">
       <c r="A216" s="0" t="s">
         <v>281</v>
       </c>
@@ -9953,7 +9954,7 @@
         <v>0.0571420619185926</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="217">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="217">
       <c r="A217" s="0" t="s">
         <v>281</v>
       </c>
@@ -9991,7 +9992,7 @@
         <v>0.057743064192322</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="218">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="218">
       <c r="A218" s="0" t="s">
         <v>281</v>
       </c>
@@ -10029,7 +10030,7 @@
         <v>0.0684263936618759</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="219">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="219">
       <c r="A219" s="0" t="s">
         <v>290</v>
       </c>
@@ -10067,7 +10068,7 @@
         <v>0.491280364615402</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="220">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="220">
       <c r="A220" s="0" t="s">
         <v>290</v>
       </c>
@@ -10105,7 +10106,7 @@
         <v>0.500419359298635</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="221">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="221">
       <c r="A221" s="0" t="s">
         <v>290</v>
       </c>
@@ -10143,7 +10144,7 @@
         <v>0.181944499915074</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="222">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="222">
       <c r="A222" s="0" t="s">
         <v>290</v>
       </c>
@@ -10181,7 +10182,7 @@
         <v>0.179012619829846</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="223">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="223">
       <c r="A223" s="0" t="s">
         <v>290</v>
       </c>
@@ -10219,7 +10220,7 @@
         <v>0.967927115102581</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="224">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="224">
       <c r="A224" s="0" t="s">
         <v>290</v>
       </c>
@@ -10257,7 +10258,7 @@
         <v>0.974359058547584</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="225">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="225">
       <c r="A225" s="0" t="s">
         <v>290</v>
       </c>
@@ -10295,7 +10296,7 @@
         <v>0.457210314672274</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="226">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="226">
       <c r="A226" s="0" t="s">
         <v>290</v>
       </c>
@@ -10333,7 +10334,7 @@
         <v>0.398746883606129</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="227">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="227">
       <c r="A227" s="0" t="s">
         <v>290</v>
       </c>
@@ -10371,7 +10372,7 @@
         <v>0.975605961891418</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="228">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="228">
       <c r="A228" s="0" t="s">
         <v>290</v>
       </c>
@@ -10409,7 +10410,7 @@
         <v>0.978764734308555</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="229">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="229">
       <c r="A229" s="0" t="s">
         <v>303</v>
       </c>
@@ -10447,7 +10448,7 @@
         <v>0.340445880175692</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="230">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="230">
       <c r="A230" s="0" t="s">
         <v>303</v>
       </c>
@@ -10485,7 +10486,7 @@
         <v>0.316283223806586</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="231">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="231">
       <c r="A231" s="0" t="s">
         <v>172</v>
       </c>
@@ -10523,7 +10524,7 @@
         <v>0.108563298549071</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="232">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="232">
       <c r="A232" s="0" t="s">
         <v>172</v>
       </c>
@@ -10561,7 +10562,7 @@
         <v>0.108626717253435</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="233">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="233">
       <c r="A233" s="0" t="s">
         <v>172</v>
       </c>
@@ -10599,7 +10600,7 @@
         <v>0.108254243572048</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="234">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="234">
       <c r="A234" s="0" t="s">
         <v>172</v>
       </c>
@@ -10637,7 +10638,7 @@
         <v>0.106590936534139</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="235">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="235">
       <c r="A235" s="0" t="s">
         <v>172</v>
       </c>
@@ -10675,7 +10676,7 @@
         <v>0.108724442416255</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="236">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="236">
       <c r="A236" s="0" t="s">
         <v>309</v>
       </c>
@@ -10713,7 +10714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="237">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="237">
       <c r="A237" s="0" t="s">
         <v>313</v>
       </c>
@@ -10751,7 +10752,7 @@
         <v>0.624078586946033</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="238">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="238">
       <c r="A238" s="0" t="s">
         <v>313</v>
       </c>
@@ -10789,7 +10790,7 @@
         <v>0.657845117179421</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="239">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="239">
       <c r="A239" s="0" t="s">
         <v>313</v>
       </c>
@@ -10827,7 +10828,7 @@
         <v>0.317767599531504</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="240">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="240">
       <c r="A240" s="0" t="s">
         <v>313</v>
       </c>
@@ -10865,7 +10866,7 @@
         <v>0.580961564881894</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="241">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="241">
       <c r="A241" s="0" t="s">
         <v>313</v>
       </c>
@@ -10903,7 +10904,7 @@
         <v>0.530346593288234</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="242">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="242">
       <c r="A242" s="0" t="s">
         <v>313</v>
       </c>
@@ -10941,7 +10942,7 @@
         <v>0.0355085508550855</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="243">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="243">
       <c r="A243" s="0" t="s">
         <v>313</v>
       </c>
@@ -10979,7 +10980,7 @@
         <v>0.00458631443771785</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="244">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="244">
       <c r="A244" s="0" t="s">
         <v>313</v>
       </c>
@@ -11017,7 +11018,7 @@
         <v>0.00574683671926198</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="245">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="245">
       <c r="A245" s="0" t="s">
         <v>313</v>
       </c>
@@ -11055,7 +11056,7 @@
         <v>0.0335060865373026</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="246">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="246">
       <c r="A246" s="0" t="s">
         <v>313</v>
       </c>
@@ -11093,7 +11094,7 @@
         <v>0.0125570776255708</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="247">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="247">
       <c r="A247" s="0" t="s">
         <v>313</v>
       </c>
@@ -11131,7 +11132,7 @@
         <v>0.00199776720136318</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="248">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="248">
       <c r="A248" s="0" t="s">
         <v>313</v>
       </c>
@@ -11169,7 +11170,7 @@
         <v>0.0328791170841907</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="249">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="249">
       <c r="A249" s="0" t="s">
         <v>313</v>
       </c>
@@ -11207,7 +11208,7 @@
         <v>0.0342600785482544</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="250">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="250">
       <c r="A250" s="0" t="s">
         <v>313</v>
       </c>
@@ -11245,7 +11246,7 @@
         <v>0.0377019455380042</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="251">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="251">
       <c r="A251" s="0" t="s">
         <v>313</v>
       </c>
@@ -11283,7 +11284,7 @@
         <v>0.0306609700929882</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="252">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="252">
       <c r="A252" s="0" t="s">
         <v>313</v>
       </c>
@@ -11321,7 +11322,7 @@
         <v>0.0219044022265644</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="253">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="253">
       <c r="A253" s="0" t="s">
         <v>313</v>
       </c>
@@ -11359,7 +11360,7 @@
         <v>0.0186958008267802</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="254">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="254">
       <c r="A254" s="0" t="s">
         <v>313</v>
       </c>
@@ -11397,7 +11398,7 @@
         <v>0.020245757753072</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="255">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="255">
       <c r="A255" s="0" t="s">
         <v>313</v>
       </c>
@@ -11435,7 +11436,7 @@
         <v>0.0221902573368183</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="256">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="256">
       <c r="A256" s="0" t="s">
         <v>313</v>
       </c>
@@ -11473,7 +11474,7 @@
         <v>0.0181587468276888</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="257">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="257">
       <c r="A257" s="0" t="s">
         <v>313</v>
       </c>
@@ -11511,7 +11512,7 @@
         <v>0.0312230315164486</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="258">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="258">
       <c r="A258" s="0" t="s">
         <v>313</v>
       </c>
@@ -11549,7 +11550,7 @@
         <v>0.0258414766558089</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="259">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="259">
       <c r="A259" s="0" t="s">
         <v>313</v>
       </c>
@@ -11587,7 +11588,7 @@
         <v>0.0306393201620711</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="260">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="260">
       <c r="A260" s="0" t="s">
         <v>313</v>
       </c>
@@ -11625,7 +11626,7 @@
         <v>0.0329653712384697</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="261">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="261">
       <c r="A261" s="0" t="s">
         <v>313</v>
       </c>
@@ -11663,7 +11664,7 @@
         <v>0.022388633857359</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="262">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="262">
       <c r="A262" s="0" t="s">
         <v>313</v>
       </c>
@@ -11701,7 +11702,7 @@
         <v>0.0574840268038024</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="263">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="263">
       <c r="A263" s="0" t="s">
         <v>313</v>
       </c>
@@ -11739,7 +11740,7 @@
         <v>0.0481139038887378</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="264">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="264">
       <c r="A264" s="0" t="s">
         <v>313</v>
       </c>
@@ -11777,7 +11778,7 @@
         <v>0.0542245148810124</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="265">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="265">
       <c r="A265" s="0" t="s">
         <v>313</v>
       </c>
@@ -11815,7 +11816,7 @@
         <v>0.0571386104977068</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="266">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="266">
       <c r="A266" s="0" t="s">
         <v>313</v>
       </c>
@@ -11853,7 +11854,7 @@
         <v>0.0480422349318082</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="267">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="267">
       <c r="A267" s="0" t="s">
         <v>313</v>
       </c>
@@ -11891,7 +11892,7 @@
         <v>0.214820574851679</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="268">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="268">
       <c r="A268" s="0" t="s">
         <v>313</v>
       </c>
@@ -11929,7 +11930,7 @@
         <v>0.205720957384705</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="269">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="269">
       <c r="A269" s="0" t="s">
         <v>313</v>
       </c>
@@ -11967,7 +11968,7 @@
         <v>0.197801351038964</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="270">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="270">
       <c r="A270" s="0" t="s">
         <v>313</v>
       </c>
@@ -12005,7 +12006,7 @@
         <v>0.21166174257205</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="271">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="271">
       <c r="A271" s="0" t="s">
         <v>313</v>
       </c>
@@ -12043,7 +12044,7 @@
         <v>0.180598142469893</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="272">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="272">
       <c r="A272" s="0" t="s">
         <v>313</v>
       </c>
@@ -12081,7 +12082,7 @@
         <v>0.178360331396068</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="273">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="273">
       <c r="A273" s="0" t="s">
         <v>313</v>
       </c>
@@ -12119,7 +12120,7 @@
         <v>0.168034588890517</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="274">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="274">
       <c r="A274" s="0" t="s">
         <v>313</v>
       </c>
@@ -12157,7 +12158,7 @@
         <v>0.158836973082783</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="275">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="275">
       <c r="A275" s="0" t="s">
         <v>313</v>
       </c>
@@ -12195,7 +12196,7 @@
         <v>0.173665364583333</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="276">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="276">
       <c r="A276" s="0" t="s">
         <v>313</v>
       </c>
@@ -12233,7 +12234,7 @@
         <v>0.149602466331332</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="277">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="277">
       <c r="A277" s="0" t="s">
         <v>313</v>
       </c>
@@ -12271,7 +12272,7 @@
         <v>0.0549872861766066</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="278">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="278">
       <c r="A278" s="0" t="s">
         <v>313</v>
       </c>
@@ -12309,7 +12310,7 @@
         <v>0.0566141109149571</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="279">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="279">
       <c r="A279" s="0" t="s">
         <v>313</v>
       </c>
@@ -12347,7 +12348,7 @@
         <v>0.052318763326226</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="280">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="280">
       <c r="A280" s="0" t="s">
         <v>313</v>
       </c>
@@ -12385,7 +12386,7 @@
         <v>0.0566406820238825</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="281">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="281">
       <c r="A281" s="0" t="s">
         <v>313</v>
       </c>
@@ -12423,7 +12424,7 @@
         <v>0.0506219765031099</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="282">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="282">
       <c r="A282" s="0" t="s">
         <v>313</v>
       </c>
@@ -12461,7 +12462,7 @@
         <v>0.0333134841868466</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="283">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="283">
       <c r="A283" s="0" t="s">
         <v>313</v>
       </c>
@@ -12499,7 +12500,7 @@
         <v>0.0334754941781749</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="284">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="284">
       <c r="A284" s="0" t="s">
         <v>313</v>
       </c>
@@ -12537,7 +12538,7 @@
         <v>0.0313698465963567</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="285">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="285">
       <c r="A285" s="0" t="s">
         <v>313</v>
       </c>
@@ -12575,7 +12576,7 @@
         <v>0.0344996729888816</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="286">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="286">
       <c r="A286" s="0" t="s">
         <v>313</v>
       </c>
@@ -12613,7 +12614,7 @@
         <v>0.0303660565723794</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="287">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="287">
       <c r="A287" s="0" t="s">
         <v>313</v>
       </c>
@@ -12651,7 +12652,7 @@
         <v>0.0617908991094303</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="288">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="288">
       <c r="A288" s="0" t="s">
         <v>313</v>
       </c>
@@ -12689,7 +12690,7 @@
         <v>0.0569703166437678</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="289">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="289">
       <c r="A289" s="0" t="s">
         <v>313</v>
       </c>
@@ -12727,7 +12728,7 @@
         <v>0.0586747022202007</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="290">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="290">
       <c r="A290" s="0" t="s">
         <v>313</v>
       </c>
@@ -12765,7 +12766,7 @@
         <v>0.0633140820840501</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="291">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="291">
       <c r="A291" s="0" t="s">
         <v>313</v>
       </c>
@@ -12803,7 +12804,7 @@
         <v>0.0557974592629169</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="292">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="292">
       <c r="A292" s="0" t="s">
         <v>313</v>
       </c>
@@ -12841,7 +12842,7 @@
         <v>0.049164058325063</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="293">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="293">
       <c r="A293" s="0" t="s">
         <v>313</v>
       </c>
@@ -12879,7 +12880,7 @@
         <v>0.0485629335976214</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="294">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="294">
       <c r="A294" s="0" t="s">
         <v>313</v>
       </c>
@@ -12917,7 +12918,7 @@
         <v>0.0483675655535373</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="295">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="295">
       <c r="A295" s="0" t="s">
         <v>313</v>
       </c>
@@ -12955,7 +12956,7 @@
         <v>0.051052122076731</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="296">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="296">
       <c r="A296" s="0" t="s">
         <v>313</v>
       </c>
@@ -12993,7 +12994,7 @@
         <v>0.0422362217203534</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="297">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="297">
       <c r="A297" s="0" t="s">
         <v>313</v>
       </c>
@@ -13031,7 +13032,7 @@
         <v>0.0385808155244412</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="298">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="298">
       <c r="A298" s="0" t="s">
         <v>313</v>
       </c>
@@ -13069,7 +13070,7 @@
         <v>0.0306528305272287</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="299">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="299">
       <c r="A299" s="0" t="s">
         <v>313</v>
       </c>
@@ -13107,7 +13108,7 @@
         <v>0.0219101783347593</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="300">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="300">
       <c r="A300" s="0" t="s">
         <v>313</v>
       </c>
@@ -13145,7 +13146,7 @@
         <v>0.0169142520958965</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="301">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="301">
       <c r="A301" s="0" t="s">
         <v>313</v>
       </c>
@@ -13183,7 +13184,7 @@
         <v>0.0321771834517342</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="302">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="302">
       <c r="A302" s="0" t="s">
         <v>313</v>
       </c>
@@ -13221,7 +13222,7 @@
         <v>0.0254407536974819</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="303">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="303">
       <c r="A303" s="0" t="s">
         <v>313</v>
       </c>
@@ -13259,7 +13260,7 @@
         <v>0.0579012759579545</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="304">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="304">
       <c r="A304" s="0" t="s">
         <v>313</v>
       </c>
@@ -13297,7 +13298,7 @@
         <v>0.0503567181926278</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="305">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="305">
       <c r="A305" s="0" t="s">
         <v>313</v>
       </c>
@@ -13335,7 +13336,7 @@
         <v>0.214857931531099</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="306">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="306">
       <c r="A306" s="0" t="s">
         <v>313</v>
       </c>
@@ -13373,7 +13374,7 @@
         <v>0.214199506742929</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="307">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="307">
       <c r="A307" s="0" t="s">
         <v>313</v>
       </c>
@@ -13411,7 +13412,7 @@
         <v>0.178593030900723</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="308">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="308">
       <c r="A308" s="0" t="s">
         <v>313</v>
       </c>
@@ -13449,7 +13450,7 @@
         <v>0.175432533425492</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="309">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="309">
       <c r="A309" s="0" t="s">
         <v>313</v>
       </c>
@@ -13487,7 +13488,7 @@
         <v>0.0559156721390925</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="310">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="310">
       <c r="A310" s="0" t="s">
         <v>313</v>
       </c>
@@ -13525,7 +13526,7 @@
         <v>0.0579387186629527</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="311">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="311">
       <c r="A311" s="0" t="s">
         <v>313</v>
       </c>
@@ -13563,7 +13564,7 @@
         <v>0.0348913305548858</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="312">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="312">
       <c r="A312" s="0" t="s">
         <v>313</v>
       </c>
@@ -13601,7 +13602,7 @@
         <v>0.0361552838802586</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="313">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="313">
       <c r="A313" s="0" t="s">
         <v>313</v>
       </c>
@@ -13639,7 +13640,7 @@
         <v>0.0636556820704748</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="314">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="314">
       <c r="A314" s="0" t="s">
         <v>313</v>
       </c>
@@ -13677,7 +13678,7 @@
         <v>0.0618133069099175</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="315">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="315">
       <c r="A315" s="0" t="s">
         <v>313</v>
       </c>
@@ -13715,7 +13716,7 @@
         <v>0.0539778885757641</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="316">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="316">
       <c r="A316" s="0" t="s">
         <v>313</v>
       </c>
@@ -13753,7 +13754,7 @@
         <v>0.0512403416022774</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="317">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="317">
       <c r="A317" s="0" t="s">
         <v>313</v>
       </c>
@@ -13791,7 +13792,7 @@
         <v>0.0885860306643952</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="318">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="318">
       <c r="A318" s="0" t="s">
         <v>313</v>
       </c>
@@ -13829,7 +13830,7 @@
         <v>0.067191935010277</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="319">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="319">
       <c r="A319" s="0" t="s">
         <v>313</v>
       </c>
@@ -13867,7 +13868,7 @@
         <v>0.0752094100873285</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="320">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="320">
       <c r="A320" s="0" t="s">
         <v>313</v>
       </c>
@@ -13905,7 +13906,7 @@
         <v>0.0594345066358915</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="321">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="321">
       <c r="A321" s="0" t="s">
         <v>313</v>
       </c>
@@ -13943,7 +13944,7 @@
         <v>0.0499508679986898</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="322">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="322">
       <c r="A322" s="0" t="s">
         <v>313</v>
       </c>
@@ -13981,7 +13982,7 @@
         <v>0.0526393394278974</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="323">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="323">
       <c r="A323" s="0" t="s">
         <v>313</v>
       </c>
@@ -14019,7 +14020,7 @@
         <v>0.064093874438702</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="324">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="324">
       <c r="A324" s="0" t="s">
         <v>313</v>
       </c>
@@ -14057,7 +14058,7 @@
         <v>0.067354997410668</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="325">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="325">
       <c r="A325" s="0" t="s">
         <v>313</v>
       </c>
@@ -14095,7 +14096,7 @@
         <v>0.0690963060686016</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="326">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="326">
       <c r="A326" s="0" t="s">
         <v>313</v>
       </c>
@@ -14133,7 +14134,7 @@
         <v>0.0412417742502637</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="327">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="327">
       <c r="A327" s="0" t="s">
         <v>313</v>
       </c>
@@ -14171,7 +14172,7 @@
         <v>0.0424639580602883</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="328">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="328">
       <c r="A328" s="0" t="s">
         <v>313</v>
       </c>
@@ -14209,7 +14210,7 @@
         <v>0.0454063229365585</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="329">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="329">
       <c r="A329" s="0" t="s">
         <v>313</v>
       </c>
@@ -14247,7 +14248,7 @@
         <v>0.247141276281815</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="330">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="330">
       <c r="A330" s="0" t="s">
         <v>313</v>
       </c>
@@ -14285,7 +14286,7 @@
         <v>0.337405260811413</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="331">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="331">
       <c r="A331" s="0" t="s">
         <v>313</v>
       </c>
@@ -14323,7 +14324,7 @@
         <v>0.34351914036266</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="332">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="332">
       <c r="A332" s="0" t="s">
         <v>313</v>
       </c>
@@ -14361,7 +14362,7 @@
         <v>0.229839927514346</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="333">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="333">
       <c r="A333" s="0" t="s">
         <v>313</v>
       </c>
@@ -14399,7 +14400,7 @@
         <v>0.2609497059598</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="334">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="334">
       <c r="A334" s="0" t="s">
         <v>313</v>
       </c>
@@ -14437,7 +14438,7 @@
         <v>0.2698476666398</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="335">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="335">
       <c r="A335" s="0" t="s">
         <v>313</v>
       </c>
@@ -14475,7 +14476,7 @@
         <v>0.0248381489785122</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="336">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="336">
       <c r="A336" s="0" t="s">
         <v>313</v>
       </c>
@@ -14513,7 +14514,7 @@
         <v>0.0247708283379752</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="337">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="337">
       <c r="A337" s="0" t="s">
         <v>313</v>
       </c>
@@ -14551,7 +14552,7 @@
         <v>0.0263157894736842</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="338">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="338">
       <c r="A338" s="0" t="s">
         <v>313</v>
       </c>
@@ -14589,7 +14590,7 @@
         <v>0.0416383027002496</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="339">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="339">
       <c r="A339" s="0" t="s">
         <v>313</v>
       </c>
@@ -14627,7 +14628,7 @@
         <v>0.0445879038214295</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="340">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="340">
       <c r="A340" s="0" t="s">
         <v>313</v>
       </c>
@@ -14665,7 +14666,7 @@
         <v>0.0427525622254758</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="341">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="341">
       <c r="A341" s="0" t="s">
         <v>313</v>
       </c>
@@ -14703,7 +14704,7 @@
         <v>0.0704252828716348</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="342">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="342">
       <c r="A342" s="0" t="s">
         <v>313</v>
       </c>
@@ -14741,7 +14742,7 @@
         <v>0.0777520791299641</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="343">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="343">
       <c r="A343" s="0" t="s">
         <v>313</v>
       </c>
@@ -14779,7 +14780,7 @@
         <v>0.0773911039410002</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="344">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="344">
       <c r="A344" s="0" t="s">
         <v>313</v>
       </c>
@@ -14817,7 +14818,7 @@
         <v>0.0810190498049116</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="345">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="345">
       <c r="A345" s="0" t="s">
         <v>313</v>
       </c>
@@ -14855,7 +14856,7 @@
         <v>0.0731630400504573</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="346">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="346">
       <c r="A346" s="0" t="s">
         <v>313</v>
       </c>
@@ -14893,7 +14894,7 @@
         <v>0.0733103763017052</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="347">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="347">
       <c r="A347" s="0" t="s">
         <v>313</v>
       </c>
@@ -14931,7 +14932,7 @@
         <v>0.0581694069289489</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="348">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="348">
       <c r="A348" s="0" t="s">
         <v>313</v>
       </c>
@@ -14969,7 +14970,7 @@
         <v>0.0271139705882353</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="349">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="349">
       <c r="A349" s="0" t="s">
         <v>313</v>
       </c>
@@ -15007,7 +15008,7 @@
         <v>0.021708436286622</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="350">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="350">
       <c r="A350" s="0" t="s">
         <v>313</v>
       </c>
@@ -15045,7 +15046,7 @@
         <v>0.0358180058083253</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="351">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="351">
       <c r="A351" s="0" t="s">
         <v>430</v>
       </c>
@@ -15083,7 +15084,7 @@
         <v>0.795706824796661</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="352">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="352">
       <c r="A352" s="0" t="s">
         <v>430</v>
       </c>
@@ -15121,7 +15122,7 @@
         <v>0.85769870460264</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="353">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="353">
       <c r="A353" s="0" t="s">
         <v>430</v>
       </c>
@@ -15159,7 +15160,7 @@
         <v>0.745487877274346</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="354">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="354">
       <c r="A354" s="0" t="s">
         <v>436</v>
       </c>
@@ -15197,7 +15198,7 @@
         <v>0.799800555111523</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="355">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="355">
       <c r="A355" s="0" t="s">
         <v>436</v>
       </c>
@@ -15235,7 +15236,7 @@
         <v>0.9859110637374</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="356">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="356">
       <c r="A356" s="0" t="s">
         <v>436</v>
       </c>
@@ -15273,7 +15274,7 @@
         <v>0.958286593725723</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="357">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="357">
       <c r="A357" s="0" t="s">
         <v>436</v>
       </c>
@@ -15311,7 +15312,7 @@
         <v>0.943347968141574</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="358">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="358">
       <c r="A358" s="0" t="s">
         <v>436</v>
       </c>
@@ -15349,7 +15350,7 @@
         <v>0.95854412377481</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="359">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="359">
       <c r="A359" s="0" t="s">
         <v>436</v>
       </c>
@@ -15387,7 +15388,7 @@
         <v>0.92010423894138</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="360">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="360">
       <c r="A360" s="0" t="s">
         <v>436</v>
       </c>
@@ -15425,7 +15426,7 @@
         <v>0.94517031989121</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="361">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="361">
       <c r="A361" s="0" t="s">
         <v>436</v>
       </c>
@@ -15463,7 +15464,7 @@
         <v>0.961366788213019</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="362">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="362">
       <c r="A362" s="0" t="s">
         <v>436</v>
       </c>
@@ -15501,7 +15502,7 @@
         <v>0.702810841845126</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="363">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="363">
       <c r="A363" s="0" t="s">
         <v>448</v>
       </c>
@@ -15539,7 +15540,7 @@
         <v>0.965564364645126</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="364">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="364">
       <c r="A364" s="0" t="s">
         <v>448</v>
       </c>
@@ -15577,7 +15578,7 @@
         <v>0.980023404861563</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="365">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="365">
       <c r="A365" s="0" t="s">
         <v>453</v>
       </c>
@@ -15615,7 +15616,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="366">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="366">
       <c r="A366" s="0" t="s">
         <v>453</v>
       </c>
@@ -15653,7 +15654,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="367">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="367">
       <c r="A367" s="0" t="s">
         <v>453</v>
       </c>
@@ -15691,7 +15692,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="368">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="368">
       <c r="A368" s="0" t="s">
         <v>453</v>
       </c>
@@ -15729,7 +15730,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="369">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="369">
       <c r="A369" s="0" t="s">
         <v>453</v>
       </c>
@@ -15767,7 +15768,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="370">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="370">
       <c r="A370" s="0" t="s">
         <v>453</v>
       </c>
@@ -15805,7 +15806,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="371">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="371">
       <c r="A371" s="0" t="s">
         <v>463</v>
       </c>
@@ -15843,7 +15844,7 @@
         <v>0.993999724816232</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="372">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="372">
       <c r="A372" s="0" t="s">
         <v>463</v>
       </c>
@@ -15881,7 +15882,7 @@
         <v>0.995869227506504</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="373">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="373">
       <c r="A373" s="0" t="s">
         <v>463</v>
       </c>
@@ -15919,7 +15920,7 @@
         <v>0.994675394027213</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="374">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="374">
       <c r="A374" s="0" t="s">
         <v>463</v>
       </c>
@@ -15957,7 +15958,7 @@
         <v>0.992816738321957</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="375">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="375">
       <c r="A375" s="0" t="s">
         <v>463</v>
       </c>
@@ -15995,7 +15996,7 @@
         <v>0.994760545465659</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="376">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="376">
       <c r="A376" s="0" t="s">
         <v>463</v>
       </c>
@@ -16033,7 +16034,7 @@
         <v>0.994599884634572</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="377">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="377">
       <c r="A377" s="0" t="s">
         <v>472</v>
       </c>
@@ -16071,7 +16072,7 @@
         <v>0.846549682263889</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="378">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="378">
       <c r="A378" s="0" t="s">
         <v>472</v>
       </c>
@@ -16109,7 +16110,7 @@
         <v>0.866649209249789</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="379">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="379">
       <c r="A379" s="0" t="s">
         <v>477</v>
       </c>
@@ -16147,7 +16148,7 @@
         <v>0.0207114439503861</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="380">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="380">
       <c r="A380" s="0" t="s">
         <v>477</v>
       </c>
@@ -16185,7 +16186,7 @@
         <v>0.0197541934803249</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="381">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="381">
       <c r="A381" s="0" t="s">
         <v>477</v>
       </c>
@@ -16223,7 +16224,7 @@
         <v>0.011960755493496</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="382">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="382">
       <c r="A382" s="0" t="s">
         <v>477</v>
       </c>
@@ -16261,7 +16262,7 @@
         <v>0.00911748749171137</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="383">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="383">
       <c r="A383" s="0" t="s">
         <v>477</v>
       </c>
@@ -16299,7 +16300,7 @@
         <v>0.0236347817732491</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="384">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="384">
       <c r="A384" s="0" t="s">
         <v>477</v>
       </c>
@@ -16337,7 +16338,7 @@
         <v>0.00211207545276677</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="385">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="385">
       <c r="A385" s="0" t="s">
         <v>477</v>
       </c>
@@ -16375,7 +16376,7 @@
         <v>0.00166358595194085</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="386">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="386">
       <c r="A386" s="0" t="s">
         <v>477</v>
       </c>
@@ -16413,7 +16414,7 @@
         <v>0.000930195473934594</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="387">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="387">
       <c r="A387" s="0" t="s">
         <v>477</v>
       </c>
@@ -16451,7 +16452,7 @@
         <v>0.000561594428983265</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="388">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="388">
       <c r="A388" s="0" t="s">
         <v>477</v>
       </c>
@@ -16489,7 +16490,7 @@
         <v>0.000546583850931677</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="389">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="389">
       <c r="A389" s="0" t="s">
         <v>477</v>
       </c>
@@ -16527,7 +16528,7 @@
         <v>0.0473007554199848</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="390">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="390">
       <c r="A390" s="0" t="s">
         <v>477</v>
       </c>
@@ -16565,7 +16566,7 @@
         <v>0.0324092151503319</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="391">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="391">
       <c r="A391" s="0" t="s">
         <v>477</v>
       </c>
@@ -16603,7 +16604,7 @@
         <v>0.0216238668849415</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="392">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="392">
       <c r="A392" s="0" t="s">
         <v>477</v>
       </c>
@@ -16641,7 +16642,7 @@
         <v>0.0135880379782819</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="393">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="393">
       <c r="A393" s="0" t="s">
         <v>477</v>
       </c>
@@ -16679,7 +16680,7 @@
         <v>0.012195492222211</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="394">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="394">
       <c r="A394" s="0" t="s">
         <v>477</v>
       </c>
@@ -16717,7 +16718,7 @@
         <v>0.00804319366127887</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="395">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="395">
       <c r="A395" s="0" t="s">
         <v>477</v>
       </c>
@@ -16755,7 +16756,7 @@
         <v>0.00604982206405694</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="396">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="396">
       <c r="A396" s="0" t="s">
         <v>477</v>
       </c>
@@ -16793,7 +16794,7 @@
         <v>0.00519652163465149</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="397">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="397">
       <c r="A397" s="0" t="s">
         <v>477</v>
       </c>
@@ -16831,7 +16832,7 @@
         <v>0.00312668816605824</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="398">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="398">
       <c r="A398" s="0" t="s">
         <v>477</v>
       </c>
@@ -16869,7 +16870,7 @@
         <v>0.00294746388546997</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="399">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="399">
       <c r="A399" s="0" t="s">
         <v>500</v>
       </c>
@@ -16907,7 +16908,7 @@
         <v>0.98497355359254</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="400">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="400">
       <c r="A400" s="0" t="s">
         <v>500</v>
       </c>
@@ -16945,7 +16946,7 @@
         <v>0.981498938228926</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="401">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="401">
       <c r="A401" s="0" t="s">
         <v>500</v>
       </c>
@@ -16983,7 +16984,7 @@
         <v>0.982978790088516</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="402">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="402">
       <c r="A402" s="0" t="s">
         <v>500</v>
       </c>
@@ -17021,7 +17022,7 @@
         <v>0.985836590428387</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="403">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="403">
       <c r="A403" s="0" t="s">
         <v>500</v>
       </c>
@@ -17059,7 +17060,7 @@
         <v>0.987362242498875</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="404">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="404">
       <c r="A404" s="0" t="s">
         <v>500</v>
       </c>
@@ -17097,7 +17098,7 @@
         <v>0.988541487866858</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="405">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="405">
       <c r="A405" s="0" t="s">
         <v>500</v>
       </c>
@@ -17135,7 +17136,7 @@
         <v>0.98497355359254</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="406">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="406">
       <c r="A406" s="0" t="s">
         <v>500</v>
       </c>
@@ -17173,7 +17174,7 @@
         <v>0.981498938228926</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="407">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="407">
       <c r="A407" s="0" t="s">
         <v>500</v>
       </c>
@@ -17211,7 +17212,7 @@
         <v>0.982978790088516</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="408">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="408">
       <c r="A408" s="0" t="s">
         <v>500</v>
       </c>
@@ -17249,7 +17250,7 @@
         <v>0.985836590428387</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="409">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="409">
       <c r="A409" s="0" t="s">
         <v>500</v>
       </c>
@@ -17287,7 +17288,7 @@
         <v>0.987362242498875</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="410">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="410">
       <c r="A410" s="0" t="s">
         <v>500</v>
       </c>
@@ -17325,7 +17326,7 @@
         <v>0.988541487866858</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="411">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="411">
       <c r="A411" s="0" t="s">
         <v>510</v>
       </c>
@@ -17363,12 +17364,12 @@
         <v>0.977042550577244</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="412">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="412">
       <c r="A412" s="0" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="B412" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C412" s="0" t="s">
         <v>512</v>
@@ -17401,18 +17402,18 @@
         <v>0.979268824740371</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="413">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="413">
       <c r="A413" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B413" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C413" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D413" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E413" s="0" t="n">
         <v>0.6130392</v>
@@ -17439,18 +17440,18 @@
         <v>0.228814836755222</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="414">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="414">
       <c r="A414" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B414" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C414" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D414" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E414" s="0" t="n">
         <v>0.7268219</v>
@@ -17477,18 +17478,18 @@
         <v>0.0987905262133813</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="415">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="415">
       <c r="A415" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B415" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C415" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D415" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E415" s="0" t="n">
         <v>0.7157102</v>
@@ -17515,18 +17516,18 @@
         <v>0.0987354159436747</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="416">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="416">
       <c r="A416" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B416" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C416" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D416" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E416" s="0" t="n">
         <v>0.6088972</v>
@@ -17553,18 +17554,18 @@
         <v>0.31804334261627</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="417">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="417">
       <c r="A417" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B417" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C417" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D417" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="E417" s="0" t="n">
         <v>0.6061916</v>
@@ -17591,18 +17592,18 @@
         <v>0.139545515603375</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="418">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="418">
       <c r="A418" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B418" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C418" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D418" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E418" s="0" t="n">
         <v>0.6069267</v>
@@ -17629,18 +17630,18 @@
         <v>0.136868857094983</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="419">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="419">
       <c r="A419" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B419" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C419" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D419" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E419" s="0" t="n">
         <v>0.7614683</v>
@@ -17667,18 +17668,18 @@
         <v>0.0308553605389943</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="420">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="420">
       <c r="A420" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B420" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C420" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D420" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E420" s="0" t="n">
         <v>0.7488464</v>
@@ -17705,18 +17706,18 @@
         <v>0.0450556164336482</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="421">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="421">
       <c r="A421" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B421" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C421" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D421" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E421" s="0" t="n">
         <v>0.7124239</v>
@@ -17743,18 +17744,18 @@
         <v>0.045381521051295</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="422">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="422">
       <c r="A422" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B422" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C422" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D422" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E422" s="0" t="n">
         <v>0.6031085</v>
@@ -17781,18 +17782,18 @@
         <v>0.812176569915273</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="423">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="423">
       <c r="A423" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B423" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C423" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D423" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E423" s="0" t="n">
         <v>0.602798</v>
@@ -17819,18 +17820,18 @@
         <v>0.816811289155818</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="424">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="424">
       <c r="A424" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B424" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C424" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D424" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E424" s="0" t="n">
         <v>0.606561</v>
@@ -17857,18 +17858,18 @@
         <v>0.818612114163629</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="425">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="425">
       <c r="A425" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B425" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C425" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D425" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E425" s="0" t="n">
         <v>0.7792352</v>
@@ -17895,18 +17896,18 @@
         <v>0.824306823195577</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="426">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="426">
       <c r="A426" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B426" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C426" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D426" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E426" s="0" t="n">
         <v>0.7785075</v>
@@ -17933,18 +17934,18 @@
         <v>0.824069696511755</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="427">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="427">
       <c r="A427" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B427" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C427" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D427" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E427" s="0" t="n">
         <v>0.780284</v>
@@ -17971,18 +17972,18 @@
         <v>0.823360830069718</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="428">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="428">
       <c r="A428" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B428" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C428" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D428" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E428" s="0" t="n">
         <v>-0.002365255</v>
@@ -18009,18 +18010,18 @@
         <v>0.931120728942459</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="429">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="429">
       <c r="A429" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B429" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="C429" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="D429" s="0" t="s">
         <v>537</v>
-      </c>
-      <c r="C429" s="0" t="s">
-        <v>535</v>
-      </c>
-      <c r="D429" s="0" t="s">
-        <v>536</v>
       </c>
       <c r="E429" s="0" t="n">
         <v>-0.0005345963</v>

</xml_diff>